<commit_message>
Phân quyền và thống kê
</commit_message>
<xml_diff>
--- a/DoAn_QuanLyShopThoiTrang/testThongKe.xlsx
+++ b/DoAn_QuanLyShopThoiTrang/testThongKe.xlsx
@@ -21,7 +21,7 @@
     <t>Cửa Hàng Thời Trang 360</t>
   </si>
   <si>
-    <t>Ngày 1 tháng 8 năm 2021</t>
+    <t>Ngày 2 tháng 8 năm 2021</t>
   </si>
   <si>
     <t>Thống kê bán hàng</t>
@@ -1496,11 +1496,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="\ #,##0_ [$VND]"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="29">
     <font>
@@ -1552,43 +1552,14 @@
     </font>
     <font>
       <sz val="14"/>
+      <color rgb="FFFF0000"/>
       <name val="Times New Roman"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="14"/>
-      <color rgb="FFFF0000"/>
       <name val="Times New Roman"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1600,14 +1571,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -1622,10 +1593,79 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1644,61 +1684,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
@@ -1708,6 +1693,21 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1722,7 +1722,109 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1734,31 +1836,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1770,61 +1854,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1836,43 +1878,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1890,13 +1896,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2140,6 +2140,24 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -2155,6 +2173,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -2166,26 +2199,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2208,184 +2221,171 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="25" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="26" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="23" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="25" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="24" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="9" borderId="23" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="28" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="26" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="13" borderId="27" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="28" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2426,17 +2426,18 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="178" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="178" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2445,13 +2446,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2460,19 +2461,19 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2851,7 +2852,7 @@
   </sheetPr>
   <dimension ref="A1:G253"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="115" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="115" zoomScaleNormal="120" topLeftCell="A229" workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -7236,11 +7237,14 @@
       <c r="F246" s="16"/>
       <c r="G246" s="16"/>
     </row>
-    <row r="247" spans="4:5">
-      <c r="D247" s="1" t="s">
+    <row r="247" ht="18.75" spans="1:5">
+      <c r="A247" s="8"/>
+      <c r="B247" s="8"/>
+      <c r="C247" s="8"/>
+      <c r="D247" s="8" t="s">
         <v>487</v>
       </c>
-      <c r="E247" s="18">
+      <c r="E247" s="21">
         <f>SUBTOTAL(109,Table1[Tổng doanh thu])</f>
         <v>9276000</v>
       </c>
@@ -7252,48 +7256,48 @@
       <c r="D248" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="E248" s="21"/>
+      <c r="E248" s="22"/>
     </row>
     <row r="249" ht="18.75" spans="1:5">
-      <c r="A249" s="22" t="s">
+      <c r="A249" s="23" t="s">
         <v>488</v>
       </c>
-      <c r="B249" s="23"/>
-      <c r="C249" s="24"/>
-      <c r="D249" s="25" t="s">
+      <c r="B249" s="24"/>
+      <c r="C249" s="25"/>
+      <c r="D249" s="26" t="s">
         <v>489</v>
       </c>
-      <c r="E249" s="26"/>
+      <c r="E249" s="27"/>
     </row>
     <row r="250" ht="18.75" spans="1:5">
-      <c r="A250" s="27"/>
-      <c r="B250" s="28"/>
-      <c r="C250" s="29"/>
-      <c r="D250" s="30" t="s">
+      <c r="A250" s="28"/>
+      <c r="B250" s="29"/>
+      <c r="C250" s="30"/>
+      <c r="D250" s="31" t="s">
         <v>490</v>
       </c>
-      <c r="E250" s="31"/>
+      <c r="E250" s="32"/>
     </row>
     <row r="251" ht="18.75" spans="1:5">
-      <c r="A251" s="32"/>
-      <c r="B251" s="33"/>
-      <c r="C251" s="29"/>
-      <c r="D251" s="30"/>
-      <c r="E251" s="31"/>
+      <c r="A251" s="33"/>
+      <c r="B251" s="34"/>
+      <c r="C251" s="30"/>
+      <c r="D251" s="31"/>
+      <c r="E251" s="32"/>
     </row>
     <row r="252" ht="18.75" spans="1:5">
-      <c r="A252" s="32"/>
-      <c r="B252" s="33"/>
-      <c r="C252" s="29"/>
-      <c r="D252" s="30"/>
-      <c r="E252" s="31"/>
+      <c r="A252" s="33"/>
+      <c r="B252" s="34"/>
+      <c r="C252" s="30"/>
+      <c r="D252" s="31"/>
+      <c r="E252" s="32"/>
     </row>
     <row r="253" ht="19.5" spans="1:5">
-      <c r="A253" s="34"/>
-      <c r="B253" s="35"/>
-      <c r="C253" s="36"/>
-      <c r="D253" s="37"/>
-      <c r="E253" s="38"/>
+      <c r="A253" s="35"/>
+      <c r="B253" s="36"/>
+      <c r="C253" s="37"/>
+      <c r="D253" s="38"/>
+      <c r="E253" s="39"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" insertColumns="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>

</xml_diff>